<commit_message>
back button fix for detail fragment and player
</commit_message>
<xml_diff>
--- a/PlanExcel/TestCase.xlsx
+++ b/PlanExcel/TestCase.xlsx
@@ -16,6 +16,7 @@
     <sheet name="ADMIN" sheetId="2" r:id="rId2"/>
     <sheet name="STATE" sheetId="3" r:id="rId3"/>
     <sheet name="UI, UX" sheetId="4" r:id="rId4"/>
+    <sheet name="VER" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="185">
   <si>
     <t>ID TestCase</t>
   </si>
@@ -579,6 +580,9 @@
   </si>
   <si>
     <t>Nếu tắt mạng thì có thể truy cập</t>
+  </si>
+  <si>
+    <t>Version = 1.0</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -3634,4 +3638,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>